<commit_message>
Implements AliExpressSite and first draft of Page Objects
</commit_message>
<xml_diff>
--- a/test cases/deviget-demo.xlsx
+++ b/test cases/deviget-demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/repo/aliexpress-demo/test cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4BF1761-ACA8-7C40-ADDB-102C1D93E342}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D684E995-B847-CC44-A309-572F855EDB73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11080" yWindow="-21140" windowWidth="22740" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14800" yWindow="-21140" windowWidth="18900" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="add song" sheetId="4" r:id="rId1"/>
@@ -65,14 +65,6 @@
     <t>URL: https://www.aliexpress.com</t>
   </si>
   <si>
-    <t>PopUoPage:
-closePopUpIcon: xpath="//div[contains(@class, 'dialog')]//a[.='x']"
-popUpHeader: xpath="//div[contains(@class, 'dialog')]//h4"
-SearchPage:
-searchTxt: id="search-key"
-searchBtn: css=".search-button"</t>
-  </si>
-  <si>
     <t>SearchPage:
 searchTxt: id="search-key"
 searchBtn: css=".search-button"
@@ -118,6 +110,14 @@
 mainProductImg: css=".magnifier-cover"
 availableProductsDiv: css=".product-quantity-tip"
 relatedItem: css=".may-like-item"</t>
+  </si>
+  <si>
+    <t>PopUpPage:
+closePopUpIcon: xpath="//div[contains(@class, 'dialog')]//a[.='x']"
+popUpHeader: xpath="//div[contains(@class, 'dialog')]//h4"
+SearchPage:
+searchTxt: id="search-key"
+searchBtn: css=".search-button"</t>
   </si>
 </sst>
 </file>
@@ -547,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55E53062-28D7-4895-A4C5-0E934E6B8F13}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="D2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -619,7 +619,7 @@
         <v>13</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F7" s="9"/>
     </row>
@@ -628,16 +628,16 @@
         <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="E8" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F8" s="9"/>
     </row>
@@ -646,14 +646,14 @@
         <v>3</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" s="9"/>
     </row>
@@ -662,16 +662,16 @@
         <v>4</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F10" s="9"/>
     </row>

</xml_diff>